<commit_message>
+2 +2 on 9mm
</commit_message>
<xml_diff>
--- a/changes/9mm-ammo.xlsx
+++ b/changes/9mm-ammo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834AC9C1-1E36-4216-AC3E-A7034A1F51B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA975239-31A9-4883-85E6-2D9A5682A5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,7 +1024,7 @@
   <dimension ref="A1:AJ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,11 +1732,11 @@
       <c r="D11" s="1">
         <v>0.08</v>
       </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-      <c r="F11" s="1">
-        <v>8</v>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="N11" s="1">
         <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+(U11-22)*2.5+P11/300+S11*5</f>
-        <v>30.783333333333331</v>
+        <v>27.983333333333331</v>
       </c>
       <c r="P11">
         <v>1150</v>
@@ -1784,11 +1784,11 @@
       <c r="D12" s="1">
         <v>0.09</v>
       </c>
-      <c r="E12" s="1">
-        <v>-8</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="E12">
         <v>-6</v>
+      </c>
+      <c r="F12">
+        <v>-4</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1">
@@ -1806,8 +1806,8 @@
         <v>750</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" ref="N12:N16" si="3">C12-D12*20-E12*0.8-F12*0.6-H12*5+(U12-22)*2.5+P12/300+S12*5</f>
-        <v>24.716666666666669</v>
+        <f>C12-D12*20-E12*0.8-F12*0.6-H12*5+(U12-22)*2.5+P12/300+S12*5</f>
+        <v>21.916666666666668</v>
       </c>
       <c r="P12">
         <v>1100</v>
@@ -1838,11 +1838,11 @@
       <c r="D13" s="1">
         <v>0.08</v>
       </c>
-      <c r="E13" s="1">
-        <v>-7</v>
-      </c>
-      <c r="F13" s="1">
-        <v>-7</v>
+      <c r="E13">
+        <v>-5</v>
+      </c>
+      <c r="F13">
+        <v>-5</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1">
@@ -1860,8 +1860,8 @@
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <f t="shared" si="3"/>
-        <v>23.866666666666667</v>
+        <f>C13-D13*20-E13*0.8-F13*0.6-H13*5+(U13-22)*2.5+P13/300+S13*5</f>
+        <v>21.066666666666666</v>
       </c>
       <c r="P13">
         <v>1250</v>
@@ -1892,11 +1892,11 @@
       <c r="D14" s="1">
         <v>0.1</v>
       </c>
-      <c r="E14" s="1">
-        <v>-11</v>
-      </c>
-      <c r="F14" s="1">
-        <v>-14</v>
+      <c r="E14">
+        <v>-9</v>
+      </c>
+      <c r="F14">
+        <v>-12</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
@@ -1914,8 +1914,8 @@
         <v>1500</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="3"/>
-        <v>25.016666666666669</v>
+        <f>C14-D14*20-E14*0.8-F14*0.6-H14*5+(U14-22)*2.5+P14/300+S14*5</f>
+        <v>22.216666666666665</v>
       </c>
       <c r="P14">
         <v>1100</v>
@@ -1946,11 +1946,11 @@
       <c r="D15" s="1">
         <v>0.06</v>
       </c>
-      <c r="E15" s="1">
-        <v>-13</v>
-      </c>
-      <c r="F15" s="1">
-        <v>-10</v>
+      <c r="E15">
+        <v>-11</v>
+      </c>
+      <c r="F15">
+        <v>-8</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
@@ -1968,8 +1968,8 @@
         <v>600</v>
       </c>
       <c r="N15" s="1">
-        <f t="shared" si="3"/>
-        <v>24.966666666666672</v>
+        <f>C15-D15*20-E15*0.8-F15*0.6-H15*5+(U15-22)*2.5+P15/300+S15*5</f>
+        <v>22.166666666666671</v>
       </c>
       <c r="P15">
         <v>1250</v>
@@ -2000,11 +2000,11 @@
       <c r="D16" s="1">
         <v>0.12</v>
       </c>
-      <c r="E16" s="1">
-        <v>-15</v>
-      </c>
-      <c r="F16" s="1">
-        <v>-20</v>
+      <c r="E16">
+        <v>-13</v>
+      </c>
+      <c r="F16">
+        <v>-18</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1">
@@ -2022,8 +2022,8 @@
         <v>1200</v>
       </c>
       <c r="N16" s="1">
-        <f t="shared" si="3"/>
-        <v>24.666666666666668</v>
+        <f>C16-D16*20-E16*0.8-F16*0.6-H16*5+(U16-22)*2.5+P16/300+S16*5</f>
+        <v>21.866666666666664</v>
       </c>
       <c r="P16">
         <v>950</v>
@@ -2042,7 +2042,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C11:U16">
+  <conditionalFormatting sqref="C11:D16 G11:U16">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C11&lt;&gt;C3</formula>
     </cfRule>

</xml_diff>